<commit_message>
fix bug carrega carrer fix bug chrome carga de lang
</commit_message>
<xml_diff>
--- a/geocatweb/dades/exemple_geocod_adreces.xlsx
+++ b/geocatweb/dades/exemple_geocod_adreces.xlsx
@@ -525,15 +525,13 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,7 +558,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -572,15 +570,16 @@
       <c r="D2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -592,9 +591,10 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>135</v>
       </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
@@ -603,15 +603,17 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
@@ -620,15 +622,17 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>23</v>
       </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
@@ -637,15 +641,17 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>5</v>
       </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
@@ -654,15 +660,17 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>5</v>
       </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
@@ -671,15 +679,17 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>12</v>
       </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
@@ -688,15 +698,17 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
@@ -705,15 +717,17 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>7</v>
       </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
         <v>26</v>
       </c>
@@ -722,15 +736,17 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>9</v>
       </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>27</v>
       </c>
@@ -739,13 +755,15 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>1</v>
       </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>29</v>
       </c>
@@ -754,15 +772,17 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>5</v>
       </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>31</v>
       </c>
@@ -771,15 +791,17 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>12</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>33</v>
       </c>
@@ -788,15 +810,17 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>16</v>
       </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
@@ -805,15 +829,17 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>13</v>
       </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>36</v>
       </c>
@@ -822,15 +848,17 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>5</v>
       </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
@@ -839,15 +867,17 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>12</v>
       </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
         <v>43</v>
       </c>
@@ -856,15 +886,17 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>9</v>
       </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>45</v>
       </c>
@@ -873,12 +905,15 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>13</v>
       </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
@@ -887,12 +922,15 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>5</v>
       </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>